<commit_message>
Solucion de bugs con el inventario y las ventas
</commit_message>
<xml_diff>
--- a/Archivos/Archivos_Stock/reporte_stock.xlsx
+++ b/Archivos/Archivos_Stock/reporte_stock.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>refresco</t>
+          <t>coca</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GUI de productos y inventarios falta comprobar si esta todo bien
</commit_message>
<xml_diff>
--- a/Archivos/Archivos_Stock/reporte_stock.xlsx
+++ b/Archivos/Archivos_Stock/reporte_stock.xlsx
@@ -469,8 +469,10 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>14</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Matriz Compras 100% con matriz
</commit_message>
<xml_diff>
--- a/Archivos/Archivos_Stock/reporte_stock.xlsx
+++ b/Archivos/Archivos_Stock/reporte_stock.xlsx
@@ -469,10 +469,8 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="E2" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="3">

</xml_diff>